<commit_message>
Procurando o ultimo fechamento como data final
</commit_message>
<xml_diff>
--- a/dados_de_fechamento.xlsx
+++ b/dados_de_fechamento.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BW270"/>
+  <dimension ref="A1:BW271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -61873,6 +61873,233 @@
         <v>2.990000009536743</v>
       </c>
     </row>
+    <row r="271">
+      <c r="A271" s="2" t="n">
+        <v>45166</v>
+      </c>
+      <c r="B271" t="n">
+        <v>117121</v>
+      </c>
+      <c r="C271" t="n">
+        <v>14.21000003814697</v>
+      </c>
+      <c r="D271" t="n">
+        <v>13.52999973297119</v>
+      </c>
+      <c r="E271" t="n">
+        <v>48.27999877929688</v>
+      </c>
+      <c r="F271" t="n">
+        <v>13.47000026702881</v>
+      </c>
+      <c r="G271" t="n">
+        <v>15.3100004196167</v>
+      </c>
+      <c r="H271" t="n">
+        <v>30.76000022888184</v>
+      </c>
+      <c r="I271" t="n">
+        <v>113.5</v>
+      </c>
+      <c r="J271" t="n">
+        <v>21.79999923706055</v>
+      </c>
+      <c r="K271" t="n">
+        <v>18.69000053405762</v>
+      </c>
+      <c r="L271" t="n">
+        <v>9.659999847412109</v>
+      </c>
+      <c r="M271" t="n">
+        <v>22.59000015258789</v>
+      </c>
+      <c r="N271" t="n">
+        <v>23.77000045776367</v>
+      </c>
+      <c r="O271" t="n">
+        <v>0.9100000262260437</v>
+      </c>
+      <c r="P271" t="n">
+        <v>12.80000019073486</v>
+      </c>
+      <c r="Q271" t="n">
+        <v>3.730000019073486</v>
+      </c>
+      <c r="R271" t="n">
+        <v>19.29999923706055</v>
+      </c>
+      <c r="S271" t="n">
+        <v>12.32999992370605</v>
+      </c>
+      <c r="T271" t="n">
+        <v>34.68999862670898</v>
+      </c>
+      <c r="U271" t="n">
+        <v>8.829999923706055</v>
+      </c>
+      <c r="V271" t="n">
+        <v>10.59000015258789</v>
+      </c>
+      <c r="W271" t="n">
+        <v>17.95999908447266</v>
+      </c>
+      <c r="X271" t="n">
+        <v>2.200000047683716</v>
+      </c>
+      <c r="Y271" t="n">
+        <v>23.29000091552734</v>
+      </c>
+      <c r="Z271" t="n">
+        <v>7.849999904632568</v>
+      </c>
+      <c r="AA271" t="n">
+        <v>42.11999893188477</v>
+      </c>
+      <c r="AB271" t="n">
+        <v>36.63999938964844</v>
+      </c>
+      <c r="AC271" t="n">
+        <v>39.81999969482422</v>
+      </c>
+      <c r="AD271" t="n">
+        <v>19.02000045776367</v>
+      </c>
+      <c r="AE271" t="n">
+        <v>31.64999961853027</v>
+      </c>
+      <c r="AF271" t="n">
+        <v>23.84000015258789</v>
+      </c>
+      <c r="AG271" t="n">
+        <v>15</v>
+      </c>
+      <c r="AH271" t="n">
+        <v>25.20000076293945</v>
+      </c>
+      <c r="AI271" t="n">
+        <v>11.60999965667725</v>
+      </c>
+      <c r="AJ271" t="n">
+        <v>7.010000228881836</v>
+      </c>
+      <c r="AK271" t="n">
+        <v>8.090000152587891</v>
+      </c>
+      <c r="AL271" t="n">
+        <v>40.11999893188477</v>
+      </c>
+      <c r="AM271" t="n">
+        <v>21.18000030517578</v>
+      </c>
+      <c r="AN271" t="n">
+        <v>9.489999771118164</v>
+      </c>
+      <c r="AO271" t="n">
+        <v>27.77000045776367</v>
+      </c>
+      <c r="AP271" t="n">
+        <v>18.72999954223633</v>
+      </c>
+      <c r="AQ271" t="n">
+        <v>22.8700008392334</v>
+      </c>
+      <c r="AR271" t="n">
+        <v>6.420000076293945</v>
+      </c>
+      <c r="AS271" t="n">
+        <v>16.70000076293945</v>
+      </c>
+      <c r="AT271" t="n">
+        <v>2.930000066757202</v>
+      </c>
+      <c r="AU271" t="n">
+        <v>6.730000019073486</v>
+      </c>
+      <c r="AV271" t="n">
+        <v>11.97999954223633</v>
+      </c>
+      <c r="AW271" t="n">
+        <v>25.8799991607666</v>
+      </c>
+      <c r="AX271" t="n">
+        <v>10.55000019073486</v>
+      </c>
+      <c r="AY271" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AZ271" t="n">
+        <v>35.40000152587891</v>
+      </c>
+      <c r="BA271" t="n">
+        <v>32.33000183105469</v>
+      </c>
+      <c r="BB271" t="n">
+        <v>6.309999942779541</v>
+      </c>
+      <c r="BC271" t="n">
+        <v>46.68999862670898</v>
+      </c>
+      <c r="BD271" t="n">
+        <v>3.680000066757202</v>
+      </c>
+      <c r="BE271" t="n">
+        <v>26.92000007629395</v>
+      </c>
+      <c r="BF271" t="n">
+        <v>22.75</v>
+      </c>
+      <c r="BG271" t="n">
+        <v>12.3100004196167</v>
+      </c>
+      <c r="BH271" t="n">
+        <v>62.86000061035156</v>
+      </c>
+      <c r="BI271" t="n">
+        <v>27.17000007629395</v>
+      </c>
+      <c r="BJ271" t="n">
+        <v>59.02999877929688</v>
+      </c>
+      <c r="BK271" t="n">
+        <v>107.0999984741211</v>
+      </c>
+      <c r="BL271" t="n">
+        <v>11.34000015258789</v>
+      </c>
+      <c r="BM271" t="n">
+        <v>25.25</v>
+      </c>
+      <c r="BN271" t="n">
+        <v>18.61000061035156</v>
+      </c>
+      <c r="BO271" t="n">
+        <v>6.880000114440918</v>
+      </c>
+      <c r="BP271" t="n">
+        <v>62.95999908447266</v>
+      </c>
+      <c r="BQ271" t="n">
+        <v>42.04999923706055</v>
+      </c>
+      <c r="BR271" t="n">
+        <v>36.61999893188477</v>
+      </c>
+      <c r="BS271" t="n">
+        <v>20.86000061035156</v>
+      </c>
+      <c r="BT271" t="n">
+        <v>1.450000047683716</v>
+      </c>
+      <c r="BU271" t="n">
+        <v>8.920000076293945</v>
+      </c>
+      <c r="BV271" t="n">
+        <v>14.56999969482422</v>
+      </c>
+      <c r="BW271" t="n">
+        <v>2.950000047683716</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>